<commit_message>
Day 4: Solved Maximum Subarray and Intersection of Two Arrays
</commit_message>
<xml_diff>
--- a/💛DSA In JS Sheet.xlsx
+++ b/💛DSA In JS Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajkishor kumar\Desktop\DSA In Js\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC432169-9E2D-476D-94CC-7B6E1183355A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954FFF31-37D8-4A0E-8ADD-0A300B55AA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="265">
   <si>
     <t>💛 8-Week DSA In Js Calendar 💛</t>
   </si>
@@ -1110,7 +1110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1173,24 +1173,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1211,6 +1193,27 @@
     </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1532,8 +1535,8 @@
   </sheetPr>
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1545,40 +1548,40 @@
     <col min="5" max="5" width="41.33203125" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="18.77734375" style="36" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:26" ht="13.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:26" ht="13.2">
-      <c r="A3" s="34"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="33"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:26" ht="17.399999999999999">
       <c r="A4" s="1" t="s">
@@ -1599,10 +1602,10 @@
       <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="39" t="s">
+      <c r="H4" s="27" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="2"/>
@@ -1625,13 +1628,13 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="13.8">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="34" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1643,17 +1646,17 @@
       <c r="F5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="H5" s="42">
+      <c r="H5" s="30">
         <v>46006</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.8">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="25"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
@@ -1663,17 +1666,17 @@
       <c r="F6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="26" t="s">
         <v>264</v>
       </c>
-      <c r="H6" s="42">
+      <c r="H6" s="30">
         <v>46006</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.8">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="24" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="34" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1685,13 +1688,17 @@
       <c r="F7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="41"/>
+      <c r="G7" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="H7" s="29">
+        <v>46007</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="13.8">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="25"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="33"/>
       <c r="D8" s="5" t="s">
         <v>20</v>
       </c>
@@ -1701,13 +1708,17 @@
       <c r="F8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="40"/>
+      <c r="G8" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="H8" s="28">
+        <v>46007</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="13.8">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="24" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="34" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1719,13 +1730,17 @@
       <c r="F9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="40"/>
+      <c r="G9" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="H9" s="28">
+        <v>46008</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="13.8">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="25"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
@@ -1735,13 +1750,17 @@
       <c r="F10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="40"/>
+      <c r="G10" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10" s="28">
+        <v>46008</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="13.8">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="24" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="34" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1753,13 +1772,17 @@
       <c r="F11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="40"/>
+      <c r="G11" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="H11" s="28">
+        <v>46010</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="13.8">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="25"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
       <c r="D12" s="5" t="s">
         <v>31</v>
       </c>
@@ -1769,13 +1792,17 @@
       <c r="F12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="40"/>
+      <c r="G12" s="43" t="s">
+        <v>264</v>
+      </c>
+      <c r="H12" s="28">
+        <v>46010</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="13.8">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="24" t="s">
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="34" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1788,12 +1815,12 @@
         <v>14</v>
       </c>
       <c r="G13" s="8"/>
-      <c r="H13" s="40"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:26" ht="13.8">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="25"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="33"/>
       <c r="D14" s="5" t="s">
         <v>36</v>
       </c>
@@ -1804,12 +1831,12 @@
         <v>14</v>
       </c>
       <c r="G14" s="8"/>
-      <c r="H14" s="40"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:26" ht="13.8">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="24" t="s">
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="34" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -1822,12 +1849,12 @@
         <v>14</v>
       </c>
       <c r="G15" s="8"/>
-      <c r="H15" s="40"/>
+      <c r="H15" s="28"/>
     </row>
     <row r="16" spans="1:26" ht="13.8">
-      <c r="A16" s="26"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="5" t="s">
         <v>41</v>
       </c>
@@ -1838,10 +1865,10 @@
         <v>14</v>
       </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="40"/>
+      <c r="H16" s="28"/>
     </row>
     <row r="17" spans="1:8" ht="38.25" customHeight="1">
-      <c r="A17" s="25"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="9" t="s">
         <v>43</v>
       </c>
@@ -1856,16 +1883,16 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="40"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="27.6">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="34" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1878,12 +1905,12 @@
         <v>30</v>
       </c>
       <c r="G18" s="8"/>
-      <c r="H18" s="40"/>
+      <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" ht="13.8">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="25"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="5" t="s">
         <v>51</v>
       </c>
@@ -1894,12 +1921,12 @@
         <v>14</v>
       </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="40"/>
+      <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="13.8">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="24" t="s">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="34" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1912,12 +1939,12 @@
         <v>30</v>
       </c>
       <c r="G20" s="8"/>
-      <c r="H20" s="40"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="13.8">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="5" t="s">
         <v>56</v>
       </c>
@@ -1928,12 +1955,12 @@
         <v>30</v>
       </c>
       <c r="G21" s="8"/>
-      <c r="H21" s="40"/>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:8" ht="27.6">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="24" t="s">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="34" t="s">
         <v>58</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1946,12 +1973,12 @@
         <v>30</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="H22" s="40"/>
+      <c r="H22" s="28"/>
     </row>
     <row r="23" spans="1:8" ht="30.75" customHeight="1">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="5" t="s">
         <v>61</v>
       </c>
@@ -1962,12 +1989,12 @@
         <v>30</v>
       </c>
       <c r="G23" s="8"/>
-      <c r="H23" s="40"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:8" ht="13.8">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="24" t="s">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="34" t="s">
         <v>63</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -1980,12 +2007,12 @@
         <v>66</v>
       </c>
       <c r="G24" s="8"/>
-      <c r="H24" s="40"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="1:8" ht="28.5" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="25"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="5" t="s">
         <v>67</v>
       </c>
@@ -1996,12 +2023,12 @@
         <v>30</v>
       </c>
       <c r="G25" s="8"/>
-      <c r="H25" s="40"/>
+      <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:8" ht="13.8">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="24" t="s">
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="34" t="s">
         <v>69</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -2014,12 +2041,12 @@
         <v>30</v>
       </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="40"/>
+      <c r="H26" s="28"/>
     </row>
     <row r="27" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="25"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="33"/>
       <c r="D27" s="5" t="s">
         <v>72</v>
       </c>
@@ -2030,11 +2057,11 @@
         <v>30</v>
       </c>
       <c r="G27" s="8"/>
-      <c r="H27" s="40"/>
+      <c r="H27" s="28"/>
     </row>
     <row r="28" spans="1:8" ht="41.25" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="25"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="9" t="s">
         <v>74</v>
       </c>
@@ -2048,10 +2075,10 @@
         <v>30</v>
       </c>
       <c r="G28" s="8"/>
-      <c r="H28" s="40"/>
+      <c r="H28" s="28"/>
     </row>
     <row r="29" spans="1:8" ht="45.75" customHeight="1">
-      <c r="A29" s="25"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="9" t="s">
         <v>43</v>
       </c>
@@ -2066,16 +2093,16 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="40"/>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8" ht="13.8">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="34" t="s">
         <v>81</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -2088,12 +2115,12 @@
         <v>30</v>
       </c>
       <c r="G30" s="8"/>
-      <c r="H30" s="40"/>
+      <c r="H30" s="28"/>
     </row>
     <row r="31" spans="1:8" ht="13.8">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="25"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="33"/>
       <c r="D31" s="5" t="s">
         <v>84</v>
       </c>
@@ -2104,12 +2131,12 @@
         <v>30</v>
       </c>
       <c r="G31" s="8"/>
-      <c r="H31" s="40"/>
+      <c r="H31" s="28"/>
     </row>
     <row r="32" spans="1:8" ht="13.8">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="24" t="s">
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="34" t="s">
         <v>86</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -2122,12 +2149,12 @@
         <v>30</v>
       </c>
       <c r="G32" s="8"/>
-      <c r="H32" s="40"/>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" spans="1:8" ht="13.8">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="33"/>
       <c r="D33" s="5" t="s">
         <v>89</v>
       </c>
@@ -2138,12 +2165,12 @@
         <v>14</v>
       </c>
       <c r="G33" s="8"/>
-      <c r="H33" s="40"/>
+      <c r="H33" s="28"/>
     </row>
     <row r="34" spans="1:8" ht="13.8">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="24" t="s">
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="34" t="s">
         <v>91</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -2156,12 +2183,12 @@
         <v>30</v>
       </c>
       <c r="G34" s="8"/>
-      <c r="H34" s="40"/>
+      <c r="H34" s="28"/>
     </row>
     <row r="35" spans="1:8" ht="13.8">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="25"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="33"/>
       <c r="D35" s="5" t="s">
         <v>94</v>
       </c>
@@ -2172,12 +2199,12 @@
         <v>14</v>
       </c>
       <c r="G35" s="8"/>
-      <c r="H35" s="40"/>
+      <c r="H35" s="28"/>
     </row>
     <row r="36" spans="1:8" ht="27.6">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="24" t="s">
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="34" t="s">
         <v>96</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -2190,12 +2217,12 @@
         <v>14</v>
       </c>
       <c r="G36" s="8"/>
-      <c r="H36" s="40"/>
+      <c r="H36" s="28"/>
     </row>
     <row r="37" spans="1:8" ht="13.8">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="25"/>
+      <c r="A37" s="32"/>
+      <c r="B37" s="32"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="5" t="s">
         <v>99</v>
       </c>
@@ -2206,12 +2233,12 @@
         <v>14</v>
       </c>
       <c r="G37" s="8"/>
-      <c r="H37" s="40"/>
+      <c r="H37" s="28"/>
     </row>
     <row r="38" spans="1:8" ht="13.8">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="24" t="s">
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="34" t="s">
         <v>101</v>
       </c>
       <c r="D38" s="5" t="s">
@@ -2224,12 +2251,12 @@
         <v>30</v>
       </c>
       <c r="G38" s="8"/>
-      <c r="H38" s="40"/>
+      <c r="H38" s="28"/>
     </row>
     <row r="39" spans="1:8" ht="13.8">
-      <c r="A39" s="26"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="A39" s="32"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="5" t="s">
         <v>104</v>
       </c>
@@ -2240,10 +2267,10 @@
         <v>30</v>
       </c>
       <c r="G39" s="8"/>
-      <c r="H39" s="40"/>
+      <c r="H39" s="28"/>
     </row>
     <row r="40" spans="1:8" ht="41.25" customHeight="1">
-      <c r="A40" s="25"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="9" t="s">
         <v>43</v>
       </c>
@@ -2258,16 +2285,16 @@
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="40"/>
+      <c r="H40" s="28"/>
     </row>
     <row r="41" spans="1:8" ht="13.8">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="34" t="s">
         <v>110</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -2280,12 +2307,12 @@
         <v>14</v>
       </c>
       <c r="G41" s="8"/>
-      <c r="H41" s="40"/>
+      <c r="H41" s="28"/>
     </row>
     <row r="42" spans="1:8" ht="13.8">
-      <c r="A42" s="26"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="25"/>
+      <c r="A42" s="32"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="33"/>
       <c r="D42" s="5" t="s">
         <v>113</v>
       </c>
@@ -2296,12 +2323,12 @@
         <v>14</v>
       </c>
       <c r="G42" s="8"/>
-      <c r="H42" s="40"/>
+      <c r="H42" s="28"/>
     </row>
     <row r="43" spans="1:8" ht="13.8">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="24" t="s">
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="34" t="s">
         <v>115</v>
       </c>
       <c r="D43" s="5" t="s">
@@ -2314,12 +2341,12 @@
         <v>14</v>
       </c>
       <c r="G43" s="8"/>
-      <c r="H43" s="40"/>
+      <c r="H43" s="28"/>
     </row>
     <row r="44" spans="1:8" ht="13.8">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="25"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="33"/>
       <c r="D44" s="5" t="s">
         <v>118</v>
       </c>
@@ -2330,12 +2357,12 @@
         <v>14</v>
       </c>
       <c r="G44" s="8"/>
-      <c r="H44" s="40"/>
+      <c r="H44" s="28"/>
     </row>
     <row r="45" spans="1:8" ht="27.6">
-      <c r="A45" s="26"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="24" t="s">
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="34" t="s">
         <v>120</v>
       </c>
       <c r="D45" s="5" t="s">
@@ -2348,12 +2375,12 @@
         <v>30</v>
       </c>
       <c r="G45" s="8"/>
-      <c r="H45" s="40"/>
+      <c r="H45" s="28"/>
     </row>
     <row r="46" spans="1:8" ht="13.8">
-      <c r="A46" s="26"/>
-      <c r="B46" s="26"/>
-      <c r="C46" s="25"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="33"/>
       <c r="D46" s="5" t="s">
         <v>123</v>
       </c>
@@ -2364,12 +2391,12 @@
         <v>14</v>
       </c>
       <c r="G46" s="8"/>
-      <c r="H46" s="40"/>
+      <c r="H46" s="28"/>
     </row>
     <row r="47" spans="1:8" ht="13.8">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="24" t="s">
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="34" t="s">
         <v>125</v>
       </c>
       <c r="D47" s="5" t="s">
@@ -2382,12 +2409,12 @@
         <v>14</v>
       </c>
       <c r="G47" s="8"/>
-      <c r="H47" s="40"/>
+      <c r="H47" s="28"/>
     </row>
     <row r="48" spans="1:8" ht="13.8">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="25"/>
+      <c r="A48" s="32"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="33"/>
       <c r="D48" s="5" t="s">
         <v>128</v>
       </c>
@@ -2398,11 +2425,11 @@
         <v>14</v>
       </c>
       <c r="G48" s="8"/>
-      <c r="H48" s="40"/>
+      <c r="H48" s="28"/>
     </row>
     <row r="49" spans="1:8" ht="47.25" customHeight="1">
-      <c r="A49" s="26"/>
-      <c r="B49" s="26"/>
+      <c r="A49" s="32"/>
+      <c r="B49" s="32"/>
       <c r="C49" s="4" t="s">
         <v>130</v>
       </c>
@@ -2416,11 +2443,11 @@
         <v>30</v>
       </c>
       <c r="G49" s="8"/>
-      <c r="H49" s="40"/>
+      <c r="H49" s="28"/>
     </row>
     <row r="50" spans="1:8" ht="47.25" customHeight="1">
-      <c r="A50" s="26"/>
-      <c r="B50" s="25"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="4" t="s">
         <v>133</v>
       </c>
@@ -2434,10 +2461,10 @@
         <v>30</v>
       </c>
       <c r="G50" s="8"/>
-      <c r="H50" s="40"/>
+      <c r="H50" s="28"/>
     </row>
     <row r="51" spans="1:8" ht="41.25" customHeight="1">
-      <c r="A51" s="25"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="9" t="s">
         <v>43</v>
       </c>
@@ -2452,16 +2479,16 @@
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
-      <c r="H51" s="40"/>
+      <c r="H51" s="28"/>
     </row>
     <row r="52" spans="1:8" ht="13.8">
-      <c r="A52" s="27" t="s">
+      <c r="A52" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="34" t="s">
         <v>140</v>
       </c>
       <c r="D52" s="5" t="s">
@@ -2474,12 +2501,12 @@
         <v>14</v>
       </c>
       <c r="G52" s="8"/>
-      <c r="H52" s="40"/>
+      <c r="H52" s="28"/>
     </row>
     <row r="53" spans="1:8" ht="13.8">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="25"/>
+      <c r="A53" s="32"/>
+      <c r="B53" s="32"/>
+      <c r="C53" s="33"/>
       <c r="D53" s="5" t="s">
         <v>143</v>
       </c>
@@ -2490,12 +2517,12 @@
         <v>30</v>
       </c>
       <c r="G53" s="8"/>
-      <c r="H53" s="40"/>
+      <c r="H53" s="28"/>
     </row>
     <row r="54" spans="1:8" ht="13.8">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="24" t="s">
+      <c r="A54" s="32"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="34" t="s">
         <v>145</v>
       </c>
       <c r="D54" s="5" t="s">
@@ -2508,12 +2535,12 @@
         <v>14</v>
       </c>
       <c r="G54" s="8"/>
-      <c r="H54" s="40"/>
+      <c r="H54" s="28"/>
     </row>
     <row r="55" spans="1:8" ht="27.6">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="25"/>
+      <c r="A55" s="32"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="33"/>
       <c r="D55" s="5" t="s">
         <v>148</v>
       </c>
@@ -2524,12 +2551,12 @@
         <v>30</v>
       </c>
       <c r="G55" s="8"/>
-      <c r="H55" s="40"/>
+      <c r="H55" s="28"/>
     </row>
     <row r="56" spans="1:8" ht="13.8">
-      <c r="A56" s="26"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="24" t="s">
+      <c r="A56" s="32"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="34" t="s">
         <v>150</v>
       </c>
       <c r="D56" s="5" t="s">
@@ -2542,12 +2569,12 @@
         <v>30</v>
       </c>
       <c r="G56" s="8"/>
-      <c r="H56" s="40"/>
+      <c r="H56" s="28"/>
     </row>
     <row r="57" spans="1:8" ht="13.8">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="25"/>
+      <c r="A57" s="32"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="33"/>
       <c r="D57" s="5" t="s">
         <v>153</v>
       </c>
@@ -2558,12 +2585,12 @@
         <v>30</v>
       </c>
       <c r="G57" s="8"/>
-      <c r="H57" s="40"/>
+      <c r="H57" s="28"/>
     </row>
     <row r="58" spans="1:8" ht="13.8">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="24" t="s">
+      <c r="A58" s="32"/>
+      <c r="B58" s="32"/>
+      <c r="C58" s="34" t="s">
         <v>155</v>
       </c>
       <c r="D58" s="5" t="s">
@@ -2576,12 +2603,12 @@
         <v>30</v>
       </c>
       <c r="G58" s="8"/>
-      <c r="H58" s="40"/>
+      <c r="H58" s="28"/>
     </row>
     <row r="59" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A59" s="26"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="25"/>
+      <c r="A59" s="32"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="33"/>
       <c r="D59" s="5" t="s">
         <v>158</v>
       </c>
@@ -2592,12 +2619,12 @@
         <v>30</v>
       </c>
       <c r="G59" s="8"/>
-      <c r="H59" s="40"/>
+      <c r="H59" s="28"/>
     </row>
     <row r="60" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="24" t="s">
+      <c r="A60" s="32"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="34" t="s">
         <v>160</v>
       </c>
       <c r="D60" s="5" t="s">
@@ -2610,12 +2637,12 @@
         <v>30</v>
       </c>
       <c r="G60" s="8"/>
-      <c r="H60" s="40"/>
+      <c r="H60" s="28"/>
     </row>
     <row r="61" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
+      <c r="A61" s="32"/>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
       <c r="D61" s="5" t="s">
         <v>163</v>
       </c>
@@ -2626,11 +2653,11 @@
         <v>30</v>
       </c>
       <c r="G61" s="8"/>
-      <c r="H61" s="40"/>
+      <c r="H61" s="28"/>
     </row>
     <row r="62" spans="1:8" ht="30" customHeight="1">
-      <c r="A62" s="26"/>
-      <c r="B62" s="25"/>
+      <c r="A62" s="32"/>
+      <c r="B62" s="33"/>
       <c r="C62" s="9" t="s">
         <v>165</v>
       </c>
@@ -2644,10 +2671,10 @@
         <v>30</v>
       </c>
       <c r="G62" s="8"/>
-      <c r="H62" s="40"/>
+      <c r="H62" s="28"/>
     </row>
     <row r="63" spans="1:8" ht="27.75" customHeight="1">
-      <c r="A63" s="25"/>
+      <c r="A63" s="33"/>
       <c r="B63" s="9" t="s">
         <v>43</v>
       </c>
@@ -2662,16 +2689,16 @@
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
-      <c r="H63" s="40"/>
+      <c r="H63" s="28"/>
     </row>
     <row r="64" spans="1:8" ht="13.8">
-      <c r="A64" s="27" t="s">
+      <c r="A64" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="B64" s="24" t="s">
+      <c r="B64" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="34" t="s">
         <v>172</v>
       </c>
       <c r="D64" s="5" t="s">
@@ -2684,12 +2711,12 @@
         <v>14</v>
       </c>
       <c r="G64" s="8"/>
-      <c r="H64" s="40"/>
+      <c r="H64" s="28"/>
     </row>
     <row r="65" spans="1:8" ht="13.8">
-      <c r="A65" s="26"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="25"/>
+      <c r="A65" s="32"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="33"/>
       <c r="D65" s="5" t="s">
         <v>175</v>
       </c>
@@ -2700,12 +2727,12 @@
         <v>14</v>
       </c>
       <c r="G65" s="8"/>
-      <c r="H65" s="40"/>
+      <c r="H65" s="28"/>
     </row>
     <row r="66" spans="1:8" ht="13.8">
-      <c r="A66" s="26"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="24" t="s">
+      <c r="A66" s="32"/>
+      <c r="B66" s="32"/>
+      <c r="C66" s="34" t="s">
         <v>177</v>
       </c>
       <c r="D66" s="5" t="s">
@@ -2718,12 +2745,12 @@
         <v>14</v>
       </c>
       <c r="G66" s="8"/>
-      <c r="H66" s="40"/>
+      <c r="H66" s="28"/>
     </row>
     <row r="67" spans="1:8" ht="13.8">
-      <c r="A67" s="26"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="25"/>
+      <c r="A67" s="32"/>
+      <c r="B67" s="32"/>
+      <c r="C67" s="33"/>
       <c r="D67" s="5" t="s">
         <v>180</v>
       </c>
@@ -2734,12 +2761,12 @@
         <v>14</v>
       </c>
       <c r="G67" s="8"/>
-      <c r="H67" s="40"/>
+      <c r="H67" s="28"/>
     </row>
     <row r="68" spans="1:8" ht="27.6">
-      <c r="A68" s="26"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="24" t="s">
+      <c r="A68" s="32"/>
+      <c r="B68" s="32"/>
+      <c r="C68" s="34" t="s">
         <v>182</v>
       </c>
       <c r="D68" s="5" t="s">
@@ -2752,12 +2779,12 @@
         <v>30</v>
       </c>
       <c r="G68" s="8"/>
-      <c r="H68" s="40"/>
+      <c r="H68" s="28"/>
     </row>
     <row r="69" spans="1:8" ht="13.8">
-      <c r="A69" s="26"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="25"/>
+      <c r="A69" s="32"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="33"/>
       <c r="D69" s="5" t="s">
         <v>185</v>
       </c>
@@ -2768,12 +2795,12 @@
         <v>30</v>
       </c>
       <c r="G69" s="8"/>
-      <c r="H69" s="40"/>
+      <c r="H69" s="28"/>
     </row>
     <row r="70" spans="1:8" ht="13.8">
-      <c r="A70" s="26"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="24" t="s">
+      <c r="A70" s="32"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="34" t="s">
         <v>187</v>
       </c>
       <c r="D70" s="5" t="s">
@@ -2786,12 +2813,12 @@
         <v>30</v>
       </c>
       <c r="G70" s="8"/>
-      <c r="H70" s="40"/>
+      <c r="H70" s="28"/>
     </row>
     <row r="71" spans="1:8" ht="13.8">
-      <c r="A71" s="26"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="25"/>
+      <c r="A71" s="32"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="33"/>
       <c r="D71" s="5" t="s">
         <v>190</v>
       </c>
@@ -2802,11 +2829,11 @@
         <v>30</v>
       </c>
       <c r="G71" s="8"/>
-      <c r="H71" s="40"/>
+      <c r="H71" s="28"/>
     </row>
     <row r="72" spans="1:8" ht="27.6">
-      <c r="A72" s="26"/>
-      <c r="B72" s="26"/>
+      <c r="A72" s="32"/>
+      <c r="B72" s="32"/>
       <c r="C72" s="4" t="s">
         <v>192</v>
       </c>
@@ -2820,11 +2847,11 @@
         <v>30</v>
       </c>
       <c r="G72" s="8"/>
-      <c r="H72" s="40"/>
+      <c r="H72" s="28"/>
     </row>
     <row r="73" spans="1:8" ht="27.6">
-      <c r="A73" s="26"/>
-      <c r="B73" s="25"/>
+      <c r="A73" s="32"/>
+      <c r="B73" s="33"/>
       <c r="C73" s="4" t="s">
         <v>195</v>
       </c>
@@ -2838,10 +2865,10 @@
         <v>66</v>
       </c>
       <c r="G73" s="8"/>
-      <c r="H73" s="40"/>
+      <c r="H73" s="28"/>
     </row>
     <row r="74" spans="1:8" ht="36" customHeight="1">
-      <c r="A74" s="25"/>
+      <c r="A74" s="33"/>
       <c r="B74" s="9" t="s">
         <v>43</v>
       </c>
@@ -2856,13 +2883,13 @@
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
-      <c r="H74" s="40"/>
+      <c r="H74" s="28"/>
     </row>
     <row r="75" spans="1:8" ht="13.8">
-      <c r="A75" s="27" t="s">
+      <c r="A75" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="B75" s="24" t="s">
+      <c r="B75" s="34" t="s">
         <v>201</v>
       </c>
       <c r="C75" s="9" t="s">
@@ -2878,12 +2905,12 @@
         <v>30</v>
       </c>
       <c r="G75" s="8"/>
-      <c r="H75" s="40"/>
+      <c r="H75" s="28"/>
     </row>
     <row r="76" spans="1:8" ht="13.8">
-      <c r="A76" s="26"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="24" t="s">
+      <c r="A76" s="32"/>
+      <c r="B76" s="32"/>
+      <c r="C76" s="34" t="s">
         <v>205</v>
       </c>
       <c r="D76" s="5" t="s">
@@ -2896,12 +2923,12 @@
         <v>14</v>
       </c>
       <c r="G76" s="8"/>
-      <c r="H76" s="40"/>
+      <c r="H76" s="28"/>
     </row>
     <row r="77" spans="1:8" ht="13.8">
-      <c r="A77" s="26"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="25"/>
+      <c r="A77" s="32"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="33"/>
       <c r="D77" s="5" t="s">
         <v>208</v>
       </c>
@@ -2912,12 +2939,12 @@
         <v>30</v>
       </c>
       <c r="G77" s="8"/>
-      <c r="H77" s="40"/>
+      <c r="H77" s="28"/>
     </row>
     <row r="78" spans="1:8" ht="13.8">
-      <c r="A78" s="26"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="24" t="s">
+      <c r="A78" s="32"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="34" t="s">
         <v>210</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -2930,12 +2957,12 @@
         <v>30</v>
       </c>
       <c r="G78" s="8"/>
-      <c r="H78" s="40"/>
+      <c r="H78" s="28"/>
     </row>
     <row r="79" spans="1:8" ht="13.8">
-      <c r="A79" s="26"/>
-      <c r="B79" s="26"/>
-      <c r="C79" s="25"/>
+      <c r="A79" s="32"/>
+      <c r="B79" s="32"/>
+      <c r="C79" s="33"/>
       <c r="D79" s="5" t="s">
         <v>213</v>
       </c>
@@ -2946,12 +2973,12 @@
         <v>215</v>
       </c>
       <c r="G79" s="8"/>
-      <c r="H79" s="40"/>
+      <c r="H79" s="28"/>
     </row>
     <row r="80" spans="1:8" ht="13.8">
-      <c r="A80" s="26"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="24" t="s">
+      <c r="A80" s="32"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="34" t="s">
         <v>216</v>
       </c>
       <c r="D80" s="5" t="s">
@@ -2964,12 +2991,12 @@
         <v>215</v>
       </c>
       <c r="G80" s="8"/>
-      <c r="H80" s="40"/>
+      <c r="H80" s="28"/>
     </row>
     <row r="81" spans="1:8" ht="13.8">
-      <c r="A81" s="26"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="25"/>
+      <c r="A81" s="32"/>
+      <c r="B81" s="32"/>
+      <c r="C81" s="33"/>
       <c r="D81" s="5" t="s">
         <v>219</v>
       </c>
@@ -2980,11 +3007,11 @@
         <v>30</v>
       </c>
       <c r="G81" s="8"/>
-      <c r="H81" s="40"/>
+      <c r="H81" s="28"/>
     </row>
     <row r="82" spans="1:8" ht="13.8">
-      <c r="A82" s="26"/>
-      <c r="B82" s="26"/>
+      <c r="A82" s="32"/>
+      <c r="B82" s="32"/>
       <c r="C82" s="4" t="s">
         <v>221</v>
       </c>
@@ -2998,11 +3025,11 @@
         <v>30</v>
       </c>
       <c r="G82" s="8"/>
-      <c r="H82" s="40"/>
+      <c r="H82" s="28"/>
     </row>
     <row r="83" spans="1:8" ht="27.6">
-      <c r="A83" s="26"/>
-      <c r="B83" s="25"/>
+      <c r="A83" s="32"/>
+      <c r="B83" s="33"/>
       <c r="C83" s="4" t="s">
         <v>224</v>
       </c>
@@ -3014,10 +3041,10 @@
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
-      <c r="H83" s="40"/>
+      <c r="H83" s="28"/>
     </row>
     <row r="84" spans="1:8" ht="33" customHeight="1">
-      <c r="A84" s="26"/>
+      <c r="A84" s="32"/>
       <c r="B84" s="9" t="s">
         <v>43</v>
       </c>
@@ -3032,16 +3059,16 @@
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
-      <c r="H84" s="40"/>
+      <c r="H84" s="28"/>
     </row>
     <row r="85" spans="1:8" ht="13.8">
-      <c r="A85" s="27" t="s">
+      <c r="A85" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="B85" s="24" t="s">
+      <c r="B85" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="C85" s="24" t="s">
+      <c r="C85" s="34" t="s">
         <v>230</v>
       </c>
       <c r="D85" s="5" t="s">
@@ -3054,12 +3081,12 @@
         <v>14</v>
       </c>
       <c r="G85" s="8"/>
-      <c r="H85" s="40"/>
+      <c r="H85" s="28"/>
     </row>
     <row r="86" spans="1:8" ht="42" customHeight="1">
-      <c r="A86" s="26"/>
-      <c r="B86" s="26"/>
-      <c r="C86" s="25"/>
+      <c r="A86" s="32"/>
+      <c r="B86" s="32"/>
+      <c r="C86" s="33"/>
       <c r="D86" s="5" t="s">
         <v>233</v>
       </c>
@@ -3070,12 +3097,12 @@
         <v>14</v>
       </c>
       <c r="G86" s="8"/>
-      <c r="H86" s="40"/>
+      <c r="H86" s="28"/>
     </row>
     <row r="87" spans="1:8" ht="13.8">
-      <c r="A87" s="26"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="24" t="s">
+      <c r="A87" s="32"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="34" t="s">
         <v>235</v>
       </c>
       <c r="D87" s="5" t="s">
@@ -3088,12 +3115,12 @@
         <v>30</v>
       </c>
       <c r="G87" s="8"/>
-      <c r="H87" s="40"/>
+      <c r="H87" s="28"/>
     </row>
     <row r="88" spans="1:8" ht="13.8">
-      <c r="A88" s="26"/>
-      <c r="B88" s="26"/>
-      <c r="C88" s="25"/>
+      <c r="A88" s="32"/>
+      <c r="B88" s="32"/>
+      <c r="C88" s="33"/>
       <c r="D88" s="5" t="s">
         <v>238</v>
       </c>
@@ -3104,12 +3131,12 @@
         <v>30</v>
       </c>
       <c r="G88" s="8"/>
-      <c r="H88" s="40"/>
+      <c r="H88" s="28"/>
     </row>
     <row r="89" spans="1:8" ht="13.8">
-      <c r="A89" s="26"/>
-      <c r="B89" s="26"/>
-      <c r="C89" s="24" t="s">
+      <c r="A89" s="32"/>
+      <c r="B89" s="32"/>
+      <c r="C89" s="34" t="s">
         <v>240</v>
       </c>
       <c r="D89" s="5" t="s">
@@ -3122,12 +3149,12 @@
         <v>30</v>
       </c>
       <c r="G89" s="8"/>
-      <c r="H89" s="40"/>
+      <c r="H89" s="28"/>
     </row>
     <row r="90" spans="1:8" ht="13.8">
-      <c r="A90" s="26"/>
-      <c r="B90" s="26"/>
-      <c r="C90" s="25"/>
+      <c r="A90" s="32"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="33"/>
       <c r="D90" s="5" t="s">
         <v>243</v>
       </c>
@@ -3138,11 +3165,11 @@
         <v>30</v>
       </c>
       <c r="G90" s="8"/>
-      <c r="H90" s="40"/>
+      <c r="H90" s="28"/>
     </row>
     <row r="91" spans="1:8" ht="21" customHeight="1">
-      <c r="A91" s="26"/>
-      <c r="B91" s="26"/>
+      <c r="A91" s="32"/>
+      <c r="B91" s="32"/>
       <c r="C91" s="4" t="s">
         <v>245</v>
       </c>
@@ -3156,11 +3183,11 @@
         <v>30</v>
       </c>
       <c r="G91" s="8"/>
-      <c r="H91" s="40"/>
+      <c r="H91" s="28"/>
     </row>
     <row r="92" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A92" s="26"/>
-      <c r="B92" s="25"/>
+      <c r="A92" s="32"/>
+      <c r="B92" s="33"/>
       <c r="C92" s="4" t="s">
         <v>248</v>
       </c>
@@ -3174,10 +3201,10 @@
         <v>30</v>
       </c>
       <c r="G92" s="8"/>
-      <c r="H92" s="40"/>
+      <c r="H92" s="28"/>
     </row>
     <row r="93" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A93" s="26"/>
+      <c r="A93" s="32"/>
       <c r="B93" s="9" t="s">
         <v>251</v>
       </c>
@@ -3192,10 +3219,10 @@
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
-      <c r="H93" s="40"/>
+      <c r="H93" s="28"/>
     </row>
     <row r="94" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A94" s="26"/>
+      <c r="A94" s="32"/>
       <c r="B94" s="9" t="s">
         <v>254</v>
       </c>
@@ -3210,10 +3237,10 @@
       </c>
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
-      <c r="H94" s="40"/>
+      <c r="H94" s="28"/>
     </row>
     <row r="95" spans="1:8" ht="13.8">
-      <c r="A95" s="25"/>
+      <c r="A95" s="33"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
       <c r="D95" s="14"/>
@@ -6974,6 +7001,46 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="B18:B28"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="A5:A17"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
     <mergeCell ref="A64:A74"/>
     <mergeCell ref="A75:A84"/>
     <mergeCell ref="A85:A95"/>
@@ -6986,46 +7053,6 @@
     <mergeCell ref="B64:B73"/>
     <mergeCell ref="B75:B83"/>
     <mergeCell ref="B85:B92"/>
-    <mergeCell ref="A1:H3"/>
-    <mergeCell ref="A5:A17"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="B18:B28"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C76:C77"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F95">
     <cfRule type="containsBlanks" dxfId="3" priority="4">
@@ -7126,6 +7153,7 @@
     <hyperlink ref="E92" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId81"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Day 6: Solved Length of last word and Majority Element
</commit_message>
<xml_diff>
--- a/💛DSA In JS Sheet.xlsx
+++ b/💛DSA In JS Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajkishor kumar\Desktop\DSA In Js\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954FFF31-37D8-4A0E-8ADD-0A300B55AA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41910679-5649-417F-AC83-462663BC1810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="265">
   <si>
     <t>💛 8-Week DSA In Js Calendar 💛</t>
   </si>
@@ -1194,12 +1194,15 @@
     <xf numFmtId="14" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1212,9 +1215,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1535,8 +1535,8 @@
   </sheetPr>
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1552,36 +1552,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:26" ht="13.2">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="40"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:26" ht="13.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="40"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="1:26" ht="17.399999999999999">
       <c r="A4" s="1" t="s">
@@ -1628,13 +1628,13 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="13.8">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="32" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -1654,8 +1654,8 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.8">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="33"/>
       <c r="D6" s="5" t="s">
         <v>15</v>
@@ -1674,9 +1674,9 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.8">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="34" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="32" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -1688,7 +1688,7 @@
       <c r="F7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="31" t="s">
         <v>264</v>
       </c>
       <c r="H7" s="29">
@@ -1696,8 +1696,8 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.8">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="33"/>
       <c r="D8" s="5" t="s">
         <v>20</v>
@@ -1708,7 +1708,7 @@
       <c r="F8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="31" t="s">
         <v>264</v>
       </c>
       <c r="H8" s="28">
@@ -1716,9 +1716,9 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.8">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="34" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="32" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1730,7 +1730,7 @@
       <c r="F9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="43" t="s">
+      <c r="G9" s="31" t="s">
         <v>264</v>
       </c>
       <c r="H9" s="28">
@@ -1738,8 +1738,8 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.8">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="33"/>
       <c r="D10" s="5" t="s">
         <v>25</v>
@@ -1750,7 +1750,7 @@
       <c r="F10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="43" t="s">
+      <c r="G10" s="31" t="s">
         <v>264</v>
       </c>
       <c r="H10" s="28">
@@ -1758,9 +1758,9 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.8">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="34" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1772,7 +1772,7 @@
       <c r="F11" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="31" t="s">
         <v>264</v>
       </c>
       <c r="H11" s="28">
@@ -1780,8 +1780,8 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.8">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="34"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="33"/>
       <c r="D12" s="5" t="s">
         <v>31</v>
@@ -1792,7 +1792,7 @@
       <c r="F12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="31" t="s">
         <v>264</v>
       </c>
       <c r="H12" s="28">
@@ -1800,9 +1800,9 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.8">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="34" t="s">
+      <c r="A13" s="34"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="32" t="s">
         <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1814,12 +1814,16 @@
       <c r="F13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="28"/>
+      <c r="G13" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="H13" s="28">
+        <v>46010</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="13.8">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="33"/>
       <c r="D14" s="5" t="s">
         <v>36</v>
@@ -1830,13 +1834,17 @@
       <c r="F14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="28"/>
+      <c r="G14" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="H14" s="28">
+        <v>46010</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="13.8">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="34" t="s">
+      <c r="A15" s="34"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="32" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -1848,11 +1856,15 @@
       <c r="F15" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="28"/>
+      <c r="G15" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="H15" s="28">
+        <v>46011</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="13.8">
-      <c r="A16" s="32"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
       <c r="D16" s="5" t="s">
@@ -1864,8 +1876,12 @@
       <c r="F16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="28"/>
+      <c r="G16" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="H16" s="28">
+        <v>46011</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="38.25" customHeight="1">
       <c r="A17" s="33"/>
@@ -1886,13 +1902,13 @@
       <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:8" ht="27.6">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="35" t="s">
         <v>263</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="32" t="s">
         <v>48</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1908,8 +1924,8 @@
       <c r="H18" s="28"/>
     </row>
     <row r="19" spans="1:8" ht="13.8">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="34"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="33"/>
       <c r="D19" s="5" t="s">
         <v>51</v>
@@ -1924,9 +1940,9 @@
       <c r="H19" s="28"/>
     </row>
     <row r="20" spans="1:8" ht="13.8">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="34" t="s">
+      <c r="A20" s="34"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="32" t="s">
         <v>53</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -1942,8 +1958,8 @@
       <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:8" ht="13.8">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
+      <c r="A21" s="34"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="33"/>
       <c r="D21" s="5" t="s">
         <v>56</v>
@@ -1958,9 +1974,9 @@
       <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:8" ht="27.6">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="34" t="s">
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="32" t="s">
         <v>58</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1976,8 +1992,8 @@
       <c r="H22" s="28"/>
     </row>
     <row r="23" spans="1:8" ht="30.75" customHeight="1">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="33"/>
       <c r="D23" s="5" t="s">
         <v>61</v>
@@ -1992,9 +2008,9 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:8" ht="13.8">
-      <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="34" t="s">
+      <c r="A24" s="34"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="32" t="s">
         <v>63</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -2010,8 +2026,8 @@
       <c r="H24" s="28"/>
     </row>
     <row r="25" spans="1:8" ht="28.5" customHeight="1">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="34"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="33"/>
       <c r="D25" s="5" t="s">
         <v>67</v>
@@ -2026,9 +2042,9 @@
       <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:8" ht="13.8">
-      <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="34" t="s">
+      <c r="A26" s="34"/>
+      <c r="B26" s="34"/>
+      <c r="C26" s="32" t="s">
         <v>69</v>
       </c>
       <c r="D26" s="5" t="s">
@@ -2044,8 +2060,8 @@
       <c r="H26" s="28"/>
     </row>
     <row r="27" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
+      <c r="A27" s="34"/>
+      <c r="B27" s="34"/>
       <c r="C27" s="33"/>
       <c r="D27" s="5" t="s">
         <v>72</v>
@@ -2060,7 +2076,7 @@
       <c r="H27" s="28"/>
     </row>
     <row r="28" spans="1:8" ht="41.25" customHeight="1">
-      <c r="A28" s="32"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="33"/>
       <c r="C28" s="9" t="s">
         <v>74</v>
@@ -2096,13 +2112,13 @@
       <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:8" ht="13.8">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="32" t="s">
         <v>81</v>
       </c>
       <c r="D30" s="5" t="s">
@@ -2118,8 +2134,8 @@
       <c r="H30" s="28"/>
     </row>
     <row r="31" spans="1:8" ht="13.8">
-      <c r="A31" s="32"/>
-      <c r="B31" s="32"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="33"/>
       <c r="D31" s="5" t="s">
         <v>84</v>
@@ -2134,9 +2150,9 @@
       <c r="H31" s="28"/>
     </row>
     <row r="32" spans="1:8" ht="13.8">
-      <c r="A32" s="32"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="34" t="s">
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="32" t="s">
         <v>86</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -2152,8 +2168,8 @@
       <c r="H32" s="28"/>
     </row>
     <row r="33" spans="1:8" ht="13.8">
-      <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
       <c r="C33" s="33"/>
       <c r="D33" s="5" t="s">
         <v>89</v>
@@ -2168,9 +2184,9 @@
       <c r="H33" s="28"/>
     </row>
     <row r="34" spans="1:8" ht="13.8">
-      <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="34" t="s">
+      <c r="A34" s="34"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="32" t="s">
         <v>91</v>
       </c>
       <c r="D34" s="5" t="s">
@@ -2186,8 +2202,8 @@
       <c r="H34" s="28"/>
     </row>
     <row r="35" spans="1:8" ht="13.8">
-      <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="33"/>
       <c r="D35" s="5" t="s">
         <v>94</v>
@@ -2202,9 +2218,9 @@
       <c r="H35" s="28"/>
     </row>
     <row r="36" spans="1:8" ht="27.6">
-      <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="34" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="32" t="s">
         <v>96</v>
       </c>
       <c r="D36" s="5" t="s">
@@ -2220,8 +2236,8 @@
       <c r="H36" s="28"/>
     </row>
     <row r="37" spans="1:8" ht="13.8">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
+      <c r="A37" s="34"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="33"/>
       <c r="D37" s="5" t="s">
         <v>99</v>
@@ -2236,9 +2252,9 @@
       <c r="H37" s="28"/>
     </row>
     <row r="38" spans="1:8" ht="13.8">
-      <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="34" t="s">
+      <c r="A38" s="34"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="32" t="s">
         <v>101</v>
       </c>
       <c r="D38" s="5" t="s">
@@ -2254,7 +2270,7 @@
       <c r="H38" s="28"/>
     </row>
     <row r="39" spans="1:8" ht="13.8">
-      <c r="A39" s="32"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
       <c r="D39" s="5" t="s">
@@ -2288,13 +2304,13 @@
       <c r="H40" s="28"/>
     </row>
     <row r="41" spans="1:8" ht="13.8">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="34" t="s">
+      <c r="C41" s="32" t="s">
         <v>110</v>
       </c>
       <c r="D41" s="5" t="s">
@@ -2310,8 +2326,8 @@
       <c r="H41" s="28"/>
     </row>
     <row r="42" spans="1:8" ht="13.8">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="33"/>
       <c r="D42" s="5" t="s">
         <v>113</v>
@@ -2326,9 +2342,9 @@
       <c r="H42" s="28"/>
     </row>
     <row r="43" spans="1:8" ht="13.8">
-      <c r="A43" s="32"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="34" t="s">
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="32" t="s">
         <v>115</v>
       </c>
       <c r="D43" s="5" t="s">
@@ -2344,8 +2360,8 @@
       <c r="H43" s="28"/>
     </row>
     <row r="44" spans="1:8" ht="13.8">
-      <c r="A44" s="32"/>
-      <c r="B44" s="32"/>
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="33"/>
       <c r="D44" s="5" t="s">
         <v>118</v>
@@ -2360,9 +2376,9 @@
       <c r="H44" s="28"/>
     </row>
     <row r="45" spans="1:8" ht="27.6">
-      <c r="A45" s="32"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="34" t="s">
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="32" t="s">
         <v>120</v>
       </c>
       <c r="D45" s="5" t="s">
@@ -2378,8 +2394,8 @@
       <c r="H45" s="28"/>
     </row>
     <row r="46" spans="1:8" ht="13.8">
-      <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="33"/>
       <c r="D46" s="5" t="s">
         <v>123</v>
@@ -2394,9 +2410,9 @@
       <c r="H46" s="28"/>
     </row>
     <row r="47" spans="1:8" ht="13.8">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="34" t="s">
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="32" t="s">
         <v>125</v>
       </c>
       <c r="D47" s="5" t="s">
@@ -2412,8 +2428,8 @@
       <c r="H47" s="28"/>
     </row>
     <row r="48" spans="1:8" ht="13.8">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
       <c r="C48" s="33"/>
       <c r="D48" s="5" t="s">
         <v>128</v>
@@ -2428,8 +2444,8 @@
       <c r="H48" s="28"/>
     </row>
     <row r="49" spans="1:8" ht="47.25" customHeight="1">
-      <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="4" t="s">
         <v>130</v>
       </c>
@@ -2446,7 +2462,7 @@
       <c r="H49" s="28"/>
     </row>
     <row r="50" spans="1:8" ht="47.25" customHeight="1">
-      <c r="A50" s="32"/>
+      <c r="A50" s="34"/>
       <c r="B50" s="33"/>
       <c r="C50" s="4" t="s">
         <v>133</v>
@@ -2482,13 +2498,13 @@
       <c r="H51" s="28"/>
     </row>
     <row r="52" spans="1:8" ht="13.8">
-      <c r="A52" s="31" t="s">
+      <c r="A52" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="C52" s="34" t="s">
+      <c r="C52" s="32" t="s">
         <v>140</v>
       </c>
       <c r="D52" s="5" t="s">
@@ -2504,8 +2520,8 @@
       <c r="H52" s="28"/>
     </row>
     <row r="53" spans="1:8" ht="13.8">
-      <c r="A53" s="32"/>
-      <c r="B53" s="32"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
       <c r="C53" s="33"/>
       <c r="D53" s="5" t="s">
         <v>143</v>
@@ -2520,9 +2536,9 @@
       <c r="H53" s="28"/>
     </row>
     <row r="54" spans="1:8" ht="13.8">
-      <c r="A54" s="32"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="34" t="s">
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="32" t="s">
         <v>145</v>
       </c>
       <c r="D54" s="5" t="s">
@@ -2538,8 +2554,8 @@
       <c r="H54" s="28"/>
     </row>
     <row r="55" spans="1:8" ht="27.6">
-      <c r="A55" s="32"/>
-      <c r="B55" s="32"/>
+      <c r="A55" s="34"/>
+      <c r="B55" s="34"/>
       <c r="C55" s="33"/>
       <c r="D55" s="5" t="s">
         <v>148</v>
@@ -2554,9 +2570,9 @@
       <c r="H55" s="28"/>
     </row>
     <row r="56" spans="1:8" ht="13.8">
-      <c r="A56" s="32"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="34" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="32" t="s">
         <v>150</v>
       </c>
       <c r="D56" s="5" t="s">
@@ -2572,8 +2588,8 @@
       <c r="H56" s="28"/>
     </row>
     <row r="57" spans="1:8" ht="13.8">
-      <c r="A57" s="32"/>
-      <c r="B57" s="32"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="34"/>
       <c r="C57" s="33"/>
       <c r="D57" s="5" t="s">
         <v>153</v>
@@ -2588,9 +2604,9 @@
       <c r="H57" s="28"/>
     </row>
     <row r="58" spans="1:8" ht="13.8">
-      <c r="A58" s="32"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="34" t="s">
+      <c r="A58" s="34"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="32" t="s">
         <v>155</v>
       </c>
       <c r="D58" s="5" t="s">
@@ -2606,8 +2622,8 @@
       <c r="H58" s="28"/>
     </row>
     <row r="59" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A59" s="32"/>
-      <c r="B59" s="32"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
       <c r="C59" s="33"/>
       <c r="D59" s="5" t="s">
         <v>158</v>
@@ -2622,9 +2638,9 @@
       <c r="H59" s="28"/>
     </row>
     <row r="60" spans="1:8" ht="22.5" customHeight="1">
-      <c r="A60" s="32"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="34" t="s">
+      <c r="A60" s="34"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="32" t="s">
         <v>160</v>
       </c>
       <c r="D60" s="5" t="s">
@@ -2640,9 +2656,9 @@
       <c r="H60" s="28"/>
     </row>
     <row r="61" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A61" s="32"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
       <c r="D61" s="5" t="s">
         <v>163</v>
       </c>
@@ -2656,7 +2672,7 @@
       <c r="H61" s="28"/>
     </row>
     <row r="62" spans="1:8" ht="30" customHeight="1">
-      <c r="A62" s="32"/>
+      <c r="A62" s="34"/>
       <c r="B62" s="33"/>
       <c r="C62" s="9" t="s">
         <v>165</v>
@@ -2692,13 +2708,13 @@
       <c r="H63" s="28"/>
     </row>
     <row r="64" spans="1:8" ht="13.8">
-      <c r="A64" s="31" t="s">
+      <c r="A64" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="B64" s="34" t="s">
+      <c r="B64" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="C64" s="34" t="s">
+      <c r="C64" s="32" t="s">
         <v>172</v>
       </c>
       <c r="D64" s="5" t="s">
@@ -2714,8 +2730,8 @@
       <c r="H64" s="28"/>
     </row>
     <row r="65" spans="1:8" ht="13.8">
-      <c r="A65" s="32"/>
-      <c r="B65" s="32"/>
+      <c r="A65" s="34"/>
+      <c r="B65" s="34"/>
       <c r="C65" s="33"/>
       <c r="D65" s="5" t="s">
         <v>175</v>
@@ -2730,9 +2746,9 @@
       <c r="H65" s="28"/>
     </row>
     <row r="66" spans="1:8" ht="13.8">
-      <c r="A66" s="32"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="34" t="s">
+      <c r="A66" s="34"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="32" t="s">
         <v>177</v>
       </c>
       <c r="D66" s="5" t="s">
@@ -2748,8 +2764,8 @@
       <c r="H66" s="28"/>
     </row>
     <row r="67" spans="1:8" ht="13.8">
-      <c r="A67" s="32"/>
-      <c r="B67" s="32"/>
+      <c r="A67" s="34"/>
+      <c r="B67" s="34"/>
       <c r="C67" s="33"/>
       <c r="D67" s="5" t="s">
         <v>180</v>
@@ -2764,9 +2780,9 @@
       <c r="H67" s="28"/>
     </row>
     <row r="68" spans="1:8" ht="27.6">
-      <c r="A68" s="32"/>
-      <c r="B68" s="32"/>
-      <c r="C68" s="34" t="s">
+      <c r="A68" s="34"/>
+      <c r="B68" s="34"/>
+      <c r="C68" s="32" t="s">
         <v>182</v>
       </c>
       <c r="D68" s="5" t="s">
@@ -2782,8 +2798,8 @@
       <c r="H68" s="28"/>
     </row>
     <row r="69" spans="1:8" ht="13.8">
-      <c r="A69" s="32"/>
-      <c r="B69" s="32"/>
+      <c r="A69" s="34"/>
+      <c r="B69" s="34"/>
       <c r="C69" s="33"/>
       <c r="D69" s="5" t="s">
         <v>185</v>
@@ -2798,9 +2814,9 @@
       <c r="H69" s="28"/>
     </row>
     <row r="70" spans="1:8" ht="13.8">
-      <c r="A70" s="32"/>
-      <c r="B70" s="32"/>
-      <c r="C70" s="34" t="s">
+      <c r="A70" s="34"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="32" t="s">
         <v>187</v>
       </c>
       <c r="D70" s="5" t="s">
@@ -2816,8 +2832,8 @@
       <c r="H70" s="28"/>
     </row>
     <row r="71" spans="1:8" ht="13.8">
-      <c r="A71" s="32"/>
-      <c r="B71" s="32"/>
+      <c r="A71" s="34"/>
+      <c r="B71" s="34"/>
       <c r="C71" s="33"/>
       <c r="D71" s="5" t="s">
         <v>190</v>
@@ -2832,8 +2848,8 @@
       <c r="H71" s="28"/>
     </row>
     <row r="72" spans="1:8" ht="27.6">
-      <c r="A72" s="32"/>
-      <c r="B72" s="32"/>
+      <c r="A72" s="34"/>
+      <c r="B72" s="34"/>
       <c r="C72" s="4" t="s">
         <v>192</v>
       </c>
@@ -2850,7 +2866,7 @@
       <c r="H72" s="28"/>
     </row>
     <row r="73" spans="1:8" ht="27.6">
-      <c r="A73" s="32"/>
+      <c r="A73" s="34"/>
       <c r="B73" s="33"/>
       <c r="C73" s="4" t="s">
         <v>195</v>
@@ -2886,10 +2902,10 @@
       <c r="H74" s="28"/>
     </row>
     <row r="75" spans="1:8" ht="13.8">
-      <c r="A75" s="31" t="s">
+      <c r="A75" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="B75" s="34" t="s">
+      <c r="B75" s="32" t="s">
         <v>201</v>
       </c>
       <c r="C75" s="9" t="s">
@@ -2908,9 +2924,9 @@
       <c r="H75" s="28"/>
     </row>
     <row r="76" spans="1:8" ht="13.8">
-      <c r="A76" s="32"/>
-      <c r="B76" s="32"/>
-      <c r="C76" s="34" t="s">
+      <c r="A76" s="34"/>
+      <c r="B76" s="34"/>
+      <c r="C76" s="32" t="s">
         <v>205</v>
       </c>
       <c r="D76" s="5" t="s">
@@ -2926,8 +2942,8 @@
       <c r="H76" s="28"/>
     </row>
     <row r="77" spans="1:8" ht="13.8">
-      <c r="A77" s="32"/>
-      <c r="B77" s="32"/>
+      <c r="A77" s="34"/>
+      <c r="B77" s="34"/>
       <c r="C77" s="33"/>
       <c r="D77" s="5" t="s">
         <v>208</v>
@@ -2942,9 +2958,9 @@
       <c r="H77" s="28"/>
     </row>
     <row r="78" spans="1:8" ht="13.8">
-      <c r="A78" s="32"/>
-      <c r="B78" s="32"/>
-      <c r="C78" s="34" t="s">
+      <c r="A78" s="34"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="32" t="s">
         <v>210</v>
       </c>
       <c r="D78" s="5" t="s">
@@ -2960,8 +2976,8 @@
       <c r="H78" s="28"/>
     </row>
     <row r="79" spans="1:8" ht="13.8">
-      <c r="A79" s="32"/>
-      <c r="B79" s="32"/>
+      <c r="A79" s="34"/>
+      <c r="B79" s="34"/>
       <c r="C79" s="33"/>
       <c r="D79" s="5" t="s">
         <v>213</v>
@@ -2976,9 +2992,9 @@
       <c r="H79" s="28"/>
     </row>
     <row r="80" spans="1:8" ht="13.8">
-      <c r="A80" s="32"/>
-      <c r="B80" s="32"/>
-      <c r="C80" s="34" t="s">
+      <c r="A80" s="34"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="32" t="s">
         <v>216</v>
       </c>
       <c r="D80" s="5" t="s">
@@ -2994,8 +3010,8 @@
       <c r="H80" s="28"/>
     </row>
     <row r="81" spans="1:8" ht="13.8">
-      <c r="A81" s="32"/>
-      <c r="B81" s="32"/>
+      <c r="A81" s="34"/>
+      <c r="B81" s="34"/>
       <c r="C81" s="33"/>
       <c r="D81" s="5" t="s">
         <v>219</v>
@@ -3010,8 +3026,8 @@
       <c r="H81" s="28"/>
     </row>
     <row r="82" spans="1:8" ht="13.8">
-      <c r="A82" s="32"/>
-      <c r="B82" s="32"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="34"/>
       <c r="C82" s="4" t="s">
         <v>221</v>
       </c>
@@ -3028,7 +3044,7 @@
       <c r="H82" s="28"/>
     </row>
     <row r="83" spans="1:8" ht="27.6">
-      <c r="A83" s="32"/>
+      <c r="A83" s="34"/>
       <c r="B83" s="33"/>
       <c r="C83" s="4" t="s">
         <v>224</v>
@@ -3044,7 +3060,7 @@
       <c r="H83" s="28"/>
     </row>
     <row r="84" spans="1:8" ht="33" customHeight="1">
-      <c r="A84" s="32"/>
+      <c r="A84" s="34"/>
       <c r="B84" s="9" t="s">
         <v>43</v>
       </c>
@@ -3062,13 +3078,13 @@
       <c r="H84" s="28"/>
     </row>
     <row r="85" spans="1:8" ht="13.8">
-      <c r="A85" s="31" t="s">
+      <c r="A85" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="B85" s="34" t="s">
+      <c r="B85" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="C85" s="34" t="s">
+      <c r="C85" s="32" t="s">
         <v>230</v>
       </c>
       <c r="D85" s="5" t="s">
@@ -3084,8 +3100,8 @@
       <c r="H85" s="28"/>
     </row>
     <row r="86" spans="1:8" ht="42" customHeight="1">
-      <c r="A86" s="32"/>
-      <c r="B86" s="32"/>
+      <c r="A86" s="34"/>
+      <c r="B86" s="34"/>
       <c r="C86" s="33"/>
       <c r="D86" s="5" t="s">
         <v>233</v>
@@ -3100,9 +3116,9 @@
       <c r="H86" s="28"/>
     </row>
     <row r="87" spans="1:8" ht="13.8">
-      <c r="A87" s="32"/>
-      <c r="B87" s="32"/>
-      <c r="C87" s="34" t="s">
+      <c r="A87" s="34"/>
+      <c r="B87" s="34"/>
+      <c r="C87" s="32" t="s">
         <v>235</v>
       </c>
       <c r="D87" s="5" t="s">
@@ -3118,8 +3134,8 @@
       <c r="H87" s="28"/>
     </row>
     <row r="88" spans="1:8" ht="13.8">
-      <c r="A88" s="32"/>
-      <c r="B88" s="32"/>
+      <c r="A88" s="34"/>
+      <c r="B88" s="34"/>
       <c r="C88" s="33"/>
       <c r="D88" s="5" t="s">
         <v>238</v>
@@ -3134,9 +3150,9 @@
       <c r="H88" s="28"/>
     </row>
     <row r="89" spans="1:8" ht="13.8">
-      <c r="A89" s="32"/>
-      <c r="B89" s="32"/>
-      <c r="C89" s="34" t="s">
+      <c r="A89" s="34"/>
+      <c r="B89" s="34"/>
+      <c r="C89" s="32" t="s">
         <v>240</v>
       </c>
       <c r="D89" s="5" t="s">
@@ -3152,8 +3168,8 @@
       <c r="H89" s="28"/>
     </row>
     <row r="90" spans="1:8" ht="13.8">
-      <c r="A90" s="32"/>
-      <c r="B90" s="32"/>
+      <c r="A90" s="34"/>
+      <c r="B90" s="34"/>
       <c r="C90" s="33"/>
       <c r="D90" s="5" t="s">
         <v>243</v>
@@ -3168,8 +3184,8 @@
       <c r="H90" s="28"/>
     </row>
     <row r="91" spans="1:8" ht="21" customHeight="1">
-      <c r="A91" s="32"/>
-      <c r="B91" s="32"/>
+      <c r="A91" s="34"/>
+      <c r="B91" s="34"/>
       <c r="C91" s="4" t="s">
         <v>245</v>
       </c>
@@ -3186,7 +3202,7 @@
       <c r="H91" s="28"/>
     </row>
     <row r="92" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A92" s="32"/>
+      <c r="A92" s="34"/>
       <c r="B92" s="33"/>
       <c r="C92" s="4" t="s">
         <v>248</v>
@@ -3204,7 +3220,7 @@
       <c r="H92" s="28"/>
     </row>
     <row r="93" spans="1:8" ht="40.5" customHeight="1">
-      <c r="A93" s="32"/>
+      <c r="A93" s="34"/>
       <c r="B93" s="9" t="s">
         <v>251</v>
       </c>
@@ -3222,7 +3238,7 @@
       <c r="H93" s="28"/>
     </row>
     <row r="94" spans="1:8" ht="35.25" customHeight="1">
-      <c r="A94" s="32"/>
+      <c r="A94" s="34"/>
       <c r="B94" s="9" t="s">
         <v>254</v>
       </c>
@@ -7001,46 +7017,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A18:A29"/>
-    <mergeCell ref="B18:B28"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A1:H3"/>
-    <mergeCell ref="A5:A17"/>
-    <mergeCell ref="B5:B16"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
     <mergeCell ref="A64:A74"/>
     <mergeCell ref="A75:A84"/>
     <mergeCell ref="A85:A95"/>
@@ -7053,6 +7029,46 @@
     <mergeCell ref="B64:B73"/>
     <mergeCell ref="B75:B83"/>
     <mergeCell ref="B85:B92"/>
+    <mergeCell ref="A1:H3"/>
+    <mergeCell ref="A5:A17"/>
+    <mergeCell ref="B5:B16"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A18:A29"/>
+    <mergeCell ref="B18:B28"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="C76:C77"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F95">
     <cfRule type="containsBlanks" dxfId="3" priority="4">

</xml_diff>